<commit_message>
add yearly data file
</commit_message>
<xml_diff>
--- a/inst/extdata/data/scabies_data_yearly.xlsx
+++ b/inst/extdata/data/scabies_data_yearly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylieainslie/Library/CloudStorage/Dropbox/Kylie/Projects/RIVM/Projects/scabies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylieainslie/Library/CloudStorage/Dropbox/Mac/Documents/mitey/inst/extdata/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1076B7AB-0006-8D41-80CE-93F258F8D810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867DA632-D706-CC42-9130-6F3826FA3520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="17100" windowHeight="16260" activeTab="1" xr2:uid="{8D6CD6B1-3358-6844-A108-45CE514A62FB}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="17100" windowHeight="16140" xr2:uid="{8D6CD6B1-3358-6844-A108-45CE514A62FB}"/>
   </bookViews>
   <sheets>
     <sheet name="total" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="157">
   <si>
     <t>Year</t>
   </si>
@@ -504,6 +504,9 @@
   </si>
   <si>
     <t>1.02</t>
+  </si>
+  <si>
+    <t>10.2</t>
   </si>
 </sst>
 </file>
@@ -918,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69159B50-7C91-EC46-807D-C49DC9EE2A3F}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,7 +1032,12 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
+      <c r="A14" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1040,7 +1048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3A38A4-12CE-E844-B0F9-2AF7CEA07A46}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>

</xml_diff>